<commit_message>
Working on income visualizations
Began analysis of median household incomes by tenure, age, and race/ethnicity
</commit_message>
<xml_diff>
--- a/data/CPI_U_RS.xlsx
+++ b/data/CPI_U_RS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\chesterfield-market-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A473354-94C6-4FCD-AE17-304C9EDBF879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA11F9CD-B3F1-45FB-83D3-C20F6EAE07BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="4740" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPI-U-RS" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -222,6 +222,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,10 +565,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:UX11850"/>
+  <dimension ref="A1:UX11851"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -938,7 +940,7 @@
       <c r="C36" s="14"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>1982</v>
       </c>
@@ -1318,44 +1320,51 @@
       <c r="C74" s="14"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" s="7" customFormat="1" ht="117.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="19" t="s">
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="22">
+        <v>2020</v>
+      </c>
+      <c r="B75" s="23">
+        <v>381.2</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" spans="1:4" s="7" customFormat="1" ht="117.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="8"/>
-    </row>
-    <row r="76" spans="1:4" s="7" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="20" t="s">
+      <c r="B76" s="19"/>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:4" s="7" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="8"/>
-    </row>
-    <row r="77" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="21"/>
-      <c r="B77" s="21"/>
+      <c r="B77" s="20"/>
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
       <c r="C78" s="8"/>
     </row>
     <row r="79" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C79" s="8"/>
     </row>
     <row r="80" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="17"/>
       <c r="C80" s="8"/>
     </row>
     <row r="81" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="17"/>
       <c r="C81" s="8"/>
     </row>
-    <row r="82" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="18"/>
+    <row r="82" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="17"/>
       <c r="C82" s="8"/>
     </row>
-    <row r="83" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A83" s="18"/>
       <c r="C83" s="8"/>
     </row>
     <row r="84" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -36659,11 +36668,14 @@
     <row r="11850" spans="3:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C11850" s="8"/>
     </row>
+    <row r="11851" spans="3:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C11851" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="10" fitToWidth="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>